<commit_message>
V4R9A: USB, Audio circuit fix. Updated component part #s.
</commit_message>
<xml_diff>
--- a/docs/pcbs/tulip4_board_v4r9/tulipcc-bom.xlsx
+++ b/docs/pcbs/tulip4_board_v4r9/tulipcc-bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nvillar\Git\Github\nvillar\tulipcc\docs\pcbs\tulip4_board_v4r9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D05FC710-82A0-4A98-B37D-5EE821DD9007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F328FD3F-1E6A-4E0C-9B56-9BDB662F012B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4185" yWindow="21480" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="6315" yWindow="2535" windowWidth="27915" windowHeight="16815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tulipcc" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="248">
   <si>
     <t>Item</t>
   </si>
@@ -436,15 +436,6 @@
     <t>470R</t>
   </si>
   <si>
-    <t>CR0805-FX-4703ELF</t>
-  </si>
-  <si>
-    <t>652-CR0805FX-4703ELF</t>
-  </si>
-  <si>
-    <t>118-CMP1206-FX-4703ELFCT-ND</t>
-  </si>
-  <si>
     <t>R15, R16</t>
   </si>
   <si>
@@ -511,12 +502,6 @@
     <t>33K</t>
   </si>
   <si>
-    <t>652-CR0805FX-3002ELF</t>
-  </si>
-  <si>
-    <t>CR1206-FX-3002ELFCT-ND</t>
-  </si>
-  <si>
     <t>R24, R25</t>
   </si>
   <si>
@@ -751,9 +736,6 @@
     <t>688-RK10J12R0A0B</t>
   </si>
   <si>
-    <t>Tulip Creative Computer V4R9</t>
-  </si>
-  <si>
     <t>Bill of Materials</t>
   </si>
   <si>
@@ -761,12 +743,33 @@
   </si>
   <si>
     <t>865060340001</t>
+  </si>
+  <si>
+    <t>CR0805-FX-3302ELF</t>
+  </si>
+  <si>
+    <t>652-CR0805FX-3302ELF</t>
+  </si>
+  <si>
+    <t>CR0805-FX-3302ELFCT-ND</t>
+  </si>
+  <si>
+    <t>CR0805-FX-4700ELF</t>
+  </si>
+  <si>
+    <t>652-CR0805FX-4700ELF</t>
+  </si>
+  <si>
+    <t>CR0805-FX-4700ELFCT-ND</t>
+  </si>
+  <si>
+    <t>Tulip Creative Computer V4R9A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1323,19 +1326,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:J50" totalsRowShown="0">
-  <autoFilter ref="A4:J50"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A4:J50" totalsRowShown="0">
+  <autoFilter ref="A4:J50" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="Item"/>
-    <tableColumn id="2" name="Qty"/>
-    <tableColumn id="3" name="Reference(s)"/>
-    <tableColumn id="4" name="Value"/>
-    <tableColumn id="5" name="Manufacturer"/>
-    <tableColumn id="6" name="Part #" dataDxfId="0"/>
-    <tableColumn id="8" name="Supplier 1"/>
-    <tableColumn id="9" name="Supplier 1 #"/>
-    <tableColumn id="10" name="Supplier 2"/>
-    <tableColumn id="11" name="Supplier 2 #"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Item"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Qty"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Reference(s)"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Value"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Manufacturer"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Part #" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Supplier 1"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Supplier 1 #"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Supplier 2"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Supplier 2 #"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1657,7 +1660,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1669,39 +1672,39 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.625" customWidth="1"/>
+    <col min="2" max="2" width="6.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="27" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" customWidth="1"/>
-    <col min="10" max="10" width="36.85546875" customWidth="1"/>
+    <col min="8" max="8" width="23.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.75" customWidth="1"/>
+    <col min="10" max="10" width="36.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="A1" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A2" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="A2" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1880,7 +1883,7 @@
         <v>35</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="G9" t="s">
         <v>14</v>
@@ -1912,7 +1915,7 @@
         <v>35</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="G10" t="s">
         <v>14</v>
@@ -2520,19 +2523,19 @@
         <v>107</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>138</v>
+        <v>244</v>
       </c>
       <c r="G29" t="s">
         <v>14</v>
       </c>
       <c r="H29" t="s">
-        <v>139</v>
+        <v>245</v>
       </c>
       <c r="I29" t="s">
         <v>16</v>
       </c>
       <c r="J29" t="s">
-        <v>140</v>
+        <v>246</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -2543,28 +2546,28 @@
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D30" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E30" t="s">
         <v>107</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G30" t="s">
         <v>14</v>
       </c>
       <c r="H30" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I30" t="s">
         <v>16</v>
       </c>
       <c r="J30" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2575,28 +2578,28 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D31" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E31" t="s">
         <v>107</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G31" t="s">
         <v>14</v>
       </c>
       <c r="H31" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I31" t="s">
         <v>16</v>
       </c>
       <c r="J31" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -2607,28 +2610,28 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D32" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E32" t="s">
         <v>107</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G32" t="s">
         <v>14</v>
       </c>
       <c r="H32" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="I32" t="s">
         <v>16</v>
       </c>
       <c r="J32" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -2639,28 +2642,28 @@
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D33" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E33" t="s">
         <v>107</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G33" t="s">
         <v>14</v>
       </c>
       <c r="H33" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="I33" t="s">
         <v>16</v>
       </c>
       <c r="J33" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2671,28 +2674,28 @@
         <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D34" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E34" t="s">
         <v>107</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>148</v>
+        <v>241</v>
       </c>
       <c r="G34" t="s">
         <v>14</v>
       </c>
       <c r="H34" t="s">
-        <v>163</v>
+        <v>242</v>
       </c>
       <c r="I34" t="s">
         <v>16</v>
       </c>
       <c r="J34" t="s">
-        <v>164</v>
+        <v>243</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -2703,28 +2706,28 @@
         <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D35" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E35" t="s">
         <v>107</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="G35" t="s">
         <v>14</v>
       </c>
       <c r="H35" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="I35" t="s">
         <v>16</v>
       </c>
       <c r="J35" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -2735,28 +2738,28 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D36" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="E36" t="s">
         <v>107</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="G36" t="s">
         <v>14</v>
       </c>
       <c r="H36" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="I36" t="s">
         <v>16</v>
       </c>
       <c r="J36" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -2767,28 +2770,28 @@
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D37" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E37" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="G37" t="s">
         <v>14</v>
       </c>
       <c r="H37" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="I37" t="s">
         <v>16</v>
       </c>
       <c r="J37" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -2799,28 +2802,28 @@
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D38" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E38" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="G38" t="s">
         <v>14</v>
       </c>
       <c r="H38" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="I38" t="s">
         <v>16</v>
       </c>
       <c r="J38" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -2831,28 +2834,28 @@
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D39" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="E39" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="G39" t="s">
         <v>14</v>
       </c>
       <c r="H39" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="I39" t="s">
         <v>16</v>
       </c>
       <c r="J39" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -2863,28 +2866,28 @@
         <v>2</v>
       </c>
       <c r="C40" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D40" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E40" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="G40" t="s">
         <v>14</v>
       </c>
       <c r="H40" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I40" t="s">
         <v>16</v>
       </c>
       <c r="J40" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -2895,28 +2898,28 @@
         <v>1</v>
       </c>
       <c r="C41" t="s">
+        <v>190</v>
+      </c>
+      <c r="D41" t="s">
+        <v>191</v>
+      </c>
+      <c r="E41" t="s">
+        <v>192</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G41" t="s">
+        <v>14</v>
+      </c>
+      <c r="H41" t="s">
+        <v>194</v>
+      </c>
+      <c r="I41" t="s">
+        <v>16</v>
+      </c>
+      <c r="J41" t="s">
         <v>195</v>
-      </c>
-      <c r="D41" t="s">
-        <v>196</v>
-      </c>
-      <c r="E41" t="s">
-        <v>197</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="G41" t="s">
-        <v>14</v>
-      </c>
-      <c r="H41" t="s">
-        <v>199</v>
-      </c>
-      <c r="I41" t="s">
-        <v>16</v>
-      </c>
-      <c r="J41" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -2927,28 +2930,28 @@
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="D42" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="E42" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="G42" t="s">
         <v>14</v>
       </c>
       <c r="H42" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="I42" t="s">
         <v>16</v>
       </c>
       <c r="J42" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -2959,28 +2962,28 @@
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D43" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E43" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="G43" t="s">
         <v>14</v>
       </c>
       <c r="H43" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="I43" t="s">
         <v>16</v>
       </c>
       <c r="J43" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -2991,28 +2994,28 @@
         <v>1</v>
       </c>
       <c r="C44" t="s">
+        <v>205</v>
+      </c>
+      <c r="D44" t="s">
+        <v>206</v>
+      </c>
+      <c r="E44" t="s">
+        <v>207</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="G44" t="s">
+        <v>14</v>
+      </c>
+      <c r="H44" t="s">
+        <v>209</v>
+      </c>
+      <c r="I44" t="s">
+        <v>16</v>
+      </c>
+      <c r="J44" t="s">
         <v>210</v>
-      </c>
-      <c r="D44" t="s">
-        <v>211</v>
-      </c>
-      <c r="E44" t="s">
-        <v>212</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="G44" t="s">
-        <v>14</v>
-      </c>
-      <c r="H44" t="s">
-        <v>214</v>
-      </c>
-      <c r="I44" t="s">
-        <v>16</v>
-      </c>
-      <c r="J44" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -3023,16 +3026,16 @@
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D45" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E45" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="G45" t="s">
         <v>14</v>
@@ -3044,7 +3047,7 @@
         <v>16</v>
       </c>
       <c r="J45" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -3055,28 +3058,28 @@
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D46" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="E46" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="G46" t="s">
         <v>14</v>
       </c>
       <c r="H46" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="I46" t="s">
         <v>16</v>
       </c>
       <c r="J46" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -3087,28 +3090,28 @@
         <v>1</v>
       </c>
       <c r="C47" t="s">
+        <v>220</v>
+      </c>
+      <c r="D47" t="s">
+        <v>221</v>
+      </c>
+      <c r="E47" t="s">
+        <v>222</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G47" t="s">
+        <v>14</v>
+      </c>
+      <c r="H47" t="s">
+        <v>224</v>
+      </c>
+      <c r="I47" t="s">
+        <v>16</v>
+      </c>
+      <c r="J47" t="s">
         <v>225</v>
-      </c>
-      <c r="D47" t="s">
-        <v>226</v>
-      </c>
-      <c r="E47" t="s">
-        <v>227</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="G47" t="s">
-        <v>14</v>
-      </c>
-      <c r="H47" t="s">
-        <v>229</v>
-      </c>
-      <c r="I47" t="s">
-        <v>16</v>
-      </c>
-      <c r="J47" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -3119,28 +3122,28 @@
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="D48" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="E48" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="G48" t="s">
         <v>14</v>
       </c>
       <c r="H48" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="I48" t="s">
         <v>16</v>
       </c>
       <c r="J48" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -3151,28 +3154,28 @@
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D49" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="E49" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="G49" t="s">
         <v>14</v>
       </c>
       <c r="H49" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="I49" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="J49" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -3183,22 +3186,22 @@
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="D50" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="E50" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="G50" t="s">
         <v>14</v>
       </c>
       <c r="H50" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wrong part ID for the 3.5mm jacks in r9
</commit_message>
<xml_diff>
--- a/docs/pcbs/tulip4_board_v4r9/tulipcc-bom.xlsx
+++ b/docs/pcbs/tulip4_board_v4r9/tulipcc-bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nvillar\Git\Github\nvillar\tulipcc\docs\pcbs\tulip4_board_v4r9\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bwhitman/outside/tulipcc/docs/pcbs/tulip4_board_v4r9/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F328FD3F-1E6A-4E0C-9B56-9BDB662F012B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3E664A-EDF1-4845-A608-31BA59DDE2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6315" yWindow="2535" windowWidth="27915" windowHeight="16815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5780" yWindow="1940" windowWidth="32660" windowHeight="21680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tulipcc" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="247">
   <si>
     <t>Item</t>
   </si>
@@ -736,9 +736,6 @@
     <t>688-RK10J12R0A0B</t>
   </si>
   <si>
-    <t>Bill of Materials</t>
-  </si>
-  <si>
     <t>865060345007</t>
   </si>
   <si>
@@ -763,7 +760,7 @@
     <t>CR0805-FX-4700ELFCT-ND</t>
   </si>
   <si>
-    <t>Tulip Creative Computer V4R9A</t>
+    <t>490-SJ2-35863B1SMTTR</t>
   </si>
 </sst>
 </file>
@@ -774,21 +771,21 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Aptos Display"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -796,7 +793,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -804,7 +801,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -812,35 +809,35 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -848,7 +845,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -856,14 +853,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -871,14 +868,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -886,7 +883,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -894,23 +891,22 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="20"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <sz val="13"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1254,15 +1250,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1326,8 +1317,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A4:J50" totalsRowShown="0">
-  <autoFilter ref="A4:J50" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J47" totalsRowShown="0">
+  <autoFilter ref="A1:J47" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Item"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Qty"/>
@@ -1355,39 +1346,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1439,7 +1430,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1550,6 +1541,13 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -1558,13 +1556,6 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1629,31 +1620,11 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1664,1553 +1635,1527 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.625" customWidth="1"/>
-    <col min="2" max="2" width="6.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="27" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="23.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.75" customWidth="1"/>
-    <col min="10" max="10" width="36.875" customWidth="1"/>
+    <col min="8" max="8" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" customWidth="1"/>
+    <col min="10" max="10" width="36.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
       <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>11</v>
-      </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="I5" t="s">
         <v>16</v>
       </c>
       <c r="J5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>20</v>
+        <v>238</v>
       </c>
       <c r="G6" t="s">
         <v>14</v>
       </c>
       <c r="H6" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="I6" t="s">
         <v>16</v>
       </c>
       <c r="J6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>25</v>
+        <v>239</v>
       </c>
       <c r="G7" t="s">
         <v>14</v>
       </c>
       <c r="H7" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="I7" t="s">
         <v>16</v>
       </c>
       <c r="J7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
         <v>4</v>
       </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="G8" t="s">
         <v>14</v>
       </c>
       <c r="H8" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="I8" t="s">
         <v>16</v>
       </c>
       <c r="J8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>239</v>
+        <v>49</v>
       </c>
       <c r="G9" t="s">
         <v>14</v>
       </c>
       <c r="H9" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="I9" t="s">
         <v>16</v>
       </c>
       <c r="J9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>240</v>
+        <v>55</v>
       </c>
       <c r="G10" t="s">
         <v>14</v>
       </c>
       <c r="H10" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="I10" t="s">
         <v>16</v>
       </c>
       <c r="J10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="E11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" t="s">
+        <v>61</v>
+      </c>
+      <c r="I11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" t="s">
+        <v>67</v>
+      </c>
+      <c r="I12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>12</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G11" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" t="s">
-        <v>45</v>
-      </c>
-      <c r="I11" t="s">
-        <v>16</v>
-      </c>
-      <c r="J11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>8</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G12" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" t="s">
-        <v>50</v>
-      </c>
-      <c r="I12" t="s">
-        <v>16</v>
-      </c>
-      <c r="J12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>9</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="D13" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="E13" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="G13" t="s">
         <v>14</v>
       </c>
       <c r="H13" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="I13" t="s">
         <v>16</v>
       </c>
       <c r="J13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="D14" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="E14" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="G14" t="s">
         <v>14</v>
       </c>
       <c r="H14" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="I14" t="s">
         <v>16</v>
       </c>
       <c r="J14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="E15" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="G15" t="s">
         <v>14</v>
       </c>
       <c r="H15" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="I15" t="s">
         <v>16</v>
       </c>
       <c r="J15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="D16" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="E16" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="G16" t="s">
         <v>14</v>
       </c>
-      <c r="H16" t="s">
-        <v>72</v>
+      <c r="H16" s="2" t="s">
+        <v>246</v>
       </c>
       <c r="I16" t="s">
         <v>16</v>
       </c>
       <c r="J16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="D17" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="E17" t="s">
         <v>76</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="G17" t="s">
         <v>14</v>
       </c>
       <c r="H17" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="I17" t="s">
         <v>16</v>
       </c>
       <c r="J17" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E18" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" t="s">
+        <v>98</v>
+      </c>
+      <c r="I18" t="s">
+        <v>16</v>
+      </c>
+      <c r="J18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" t="s">
+        <v>103</v>
+      </c>
+      <c r="I19" t="s">
+        <v>16</v>
+      </c>
+      <c r="J19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" t="s">
+        <v>106</v>
+      </c>
+      <c r="E20" t="s">
+        <v>107</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G20" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" t="s">
+        <v>109</v>
+      </c>
+      <c r="I20" t="s">
+        <v>16</v>
+      </c>
+      <c r="J20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
         <v>2</v>
       </c>
-      <c r="C18" t="s">
-        <v>79</v>
-      </c>
-      <c r="D18" t="s">
-        <v>80</v>
-      </c>
-      <c r="E18" t="s">
-        <v>81</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" t="s">
-        <v>82</v>
-      </c>
-      <c r="I18" t="s">
-        <v>16</v>
-      </c>
-      <c r="J18" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>15</v>
-      </c>
-      <c r="B19">
-        <v>3</v>
-      </c>
-      <c r="C19" t="s">
-        <v>84</v>
-      </c>
-      <c r="D19" t="s">
-        <v>85</v>
-      </c>
-      <c r="E19" t="s">
-        <v>86</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G19" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19" t="s">
-        <v>88</v>
-      </c>
-      <c r="I19" t="s">
-        <v>16</v>
-      </c>
-      <c r="J19" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>16</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
-        <v>90</v>
-      </c>
-      <c r="D20" t="s">
-        <v>91</v>
-      </c>
-      <c r="E20" t="s">
-        <v>76</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G20" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" t="s">
-        <v>92</v>
-      </c>
-      <c r="I20" t="s">
-        <v>16</v>
-      </c>
-      <c r="J20" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>17</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
       <c r="C21" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="D21" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="E21" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="G21" t="s">
         <v>14</v>
       </c>
       <c r="H21" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="I21" t="s">
         <v>16</v>
       </c>
       <c r="J21" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="D22" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="E22" t="s">
-        <v>60</v>
+        <v>107</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="G22" t="s">
         <v>14</v>
       </c>
       <c r="H22" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="I22" t="s">
         <v>16</v>
       </c>
       <c r="J22" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B23">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="D23" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="E23" t="s">
         <v>107</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="G23" t="s">
         <v>14</v>
       </c>
       <c r="H23" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="I23" t="s">
         <v>16</v>
       </c>
       <c r="J23" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B24">
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="D24" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="E24" t="s">
         <v>107</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="G24" t="s">
         <v>14</v>
       </c>
       <c r="H24" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="I24" t="s">
         <v>16</v>
       </c>
       <c r="J24" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
       <c r="D25" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
       <c r="E25" t="s">
         <v>107</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
       <c r="G25" t="s">
         <v>14</v>
       </c>
       <c r="H25" t="s">
-        <v>119</v>
+        <v>134</v>
       </c>
       <c r="I25" t="s">
         <v>16</v>
       </c>
       <c r="J25" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="D26" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="E26" t="s">
         <v>107</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>123</v>
+        <v>243</v>
       </c>
       <c r="G26" t="s">
         <v>14</v>
       </c>
       <c r="H26" t="s">
-        <v>124</v>
+        <v>244</v>
       </c>
       <c r="I26" t="s">
         <v>16</v>
       </c>
       <c r="J26" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B27">
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="D27" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="E27" t="s">
         <v>107</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="G27" t="s">
         <v>14</v>
       </c>
       <c r="H27" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="I27" t="s">
         <v>16</v>
       </c>
       <c r="J27" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="D28" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="E28" t="s">
         <v>107</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="G28" t="s">
         <v>14</v>
       </c>
       <c r="H28" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="I28" t="s">
         <v>16</v>
       </c>
       <c r="J28" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B29">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="D29" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="E29" t="s">
         <v>107</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>244</v>
+        <v>150</v>
       </c>
       <c r="G29" t="s">
         <v>14</v>
       </c>
       <c r="H29" t="s">
-        <v>245</v>
+        <v>151</v>
       </c>
       <c r="I29" t="s">
         <v>16</v>
       </c>
       <c r="J29" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B30">
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>138</v>
+        <v>153</v>
       </c>
       <c r="D30" t="s">
-        <v>139</v>
+        <v>154</v>
       </c>
       <c r="E30" t="s">
         <v>107</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>140</v>
+        <v>155</v>
       </c>
       <c r="G30" t="s">
         <v>14</v>
       </c>
       <c r="H30" t="s">
-        <v>141</v>
+        <v>156</v>
       </c>
       <c r="I30" t="s">
         <v>16</v>
       </c>
       <c r="J30" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>143</v>
+        <v>158</v>
       </c>
       <c r="D31" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="E31" t="s">
         <v>107</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>145</v>
+        <v>240</v>
       </c>
       <c r="G31" t="s">
         <v>14</v>
       </c>
       <c r="H31" t="s">
-        <v>146</v>
+        <v>241</v>
       </c>
       <c r="I31" t="s">
         <v>16</v>
       </c>
       <c r="J31" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="D32" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="E32" t="s">
         <v>107</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="G32" t="s">
         <v>14</v>
       </c>
       <c r="H32" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="I32" t="s">
         <v>16</v>
       </c>
       <c r="J32" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="D33" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="E33" t="s">
         <v>107</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="G33" t="s">
         <v>14</v>
       </c>
       <c r="H33" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="I33" t="s">
         <v>16</v>
       </c>
       <c r="J33" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c r="D34" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="E34" t="s">
-        <v>107</v>
+        <v>172</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>241</v>
+        <v>171</v>
       </c>
       <c r="G34" t="s">
         <v>14</v>
       </c>
       <c r="H34" t="s">
-        <v>242</v>
+        <v>173</v>
       </c>
       <c r="I34" t="s">
         <v>16</v>
       </c>
       <c r="J34" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>160</v>
+        <v>175</v>
       </c>
       <c r="D35" t="s">
-        <v>161</v>
+        <v>176</v>
       </c>
       <c r="E35" t="s">
-        <v>107</v>
+        <v>177</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="G35" t="s">
         <v>14</v>
       </c>
       <c r="H35" t="s">
-        <v>163</v>
+        <v>178</v>
       </c>
       <c r="I35" t="s">
         <v>16</v>
       </c>
       <c r="J35" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>165</v>
+        <v>180</v>
       </c>
       <c r="D36" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
       <c r="E36" t="s">
-        <v>107</v>
+        <v>182</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="G36" t="s">
         <v>14</v>
       </c>
       <c r="H36" t="s">
-        <v>168</v>
+        <v>183</v>
       </c>
       <c r="I36" t="s">
         <v>16</v>
       </c>
       <c r="J36" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>170</v>
+        <v>185</v>
       </c>
       <c r="D37" t="s">
-        <v>171</v>
+        <v>186</v>
       </c>
       <c r="E37" t="s">
-        <v>172</v>
+        <v>187</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>171</v>
+        <v>186</v>
       </c>
       <c r="G37" t="s">
         <v>14</v>
       </c>
       <c r="H37" t="s">
-        <v>173</v>
+        <v>188</v>
       </c>
       <c r="I37" t="s">
         <v>16</v>
       </c>
       <c r="J37" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="D38" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="E38" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>176</v>
+        <v>193</v>
       </c>
       <c r="G38" t="s">
         <v>14</v>
       </c>
       <c r="H38" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
       <c r="I38" t="s">
         <v>16</v>
       </c>
       <c r="J38" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="D39" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="E39" t="s">
+        <v>198</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="G39" t="s">
+        <v>14</v>
+      </c>
+      <c r="H39" t="s">
+        <v>199</v>
+      </c>
+      <c r="I39" t="s">
+        <v>16</v>
+      </c>
+      <c r="J39" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>201</v>
+      </c>
+      <c r="D40" t="s">
+        <v>202</v>
+      </c>
+      <c r="E40" t="s">
         <v>182</v>
       </c>
-      <c r="F39" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="G39" t="s">
-        <v>14</v>
-      </c>
-      <c r="H39" t="s">
-        <v>183</v>
-      </c>
-      <c r="I39" t="s">
-        <v>16</v>
-      </c>
-      <c r="J39" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>36</v>
-      </c>
-      <c r="B40">
-        <v>2</v>
-      </c>
-      <c r="C40" t="s">
-        <v>185</v>
-      </c>
-      <c r="D40" t="s">
-        <v>186</v>
-      </c>
-      <c r="E40" t="s">
-        <v>187</v>
-      </c>
       <c r="F40" s="1" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
       <c r="G40" t="s">
         <v>14</v>
       </c>
       <c r="H40" t="s">
-        <v>188</v>
+        <v>203</v>
       </c>
       <c r="I40" t="s">
         <v>16</v>
       </c>
       <c r="J40" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>190</v>
+        <v>205</v>
       </c>
       <c r="D41" t="s">
-        <v>191</v>
+        <v>206</v>
       </c>
       <c r="E41" t="s">
-        <v>192</v>
+        <v>207</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="G41" t="s">
         <v>14</v>
       </c>
       <c r="H41" t="s">
-        <v>194</v>
+        <v>209</v>
       </c>
       <c r="I41" t="s">
         <v>16</v>
       </c>
       <c r="J41" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="D42" t="s">
-        <v>197</v>
+        <v>212</v>
       </c>
       <c r="E42" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>197</v>
+        <v>213</v>
       </c>
       <c r="G42" t="s">
         <v>14</v>
       </c>
       <c r="H42" t="s">
-        <v>199</v>
+        <v>88</v>
       </c>
       <c r="I42" t="s">
         <v>16</v>
       </c>
       <c r="J42" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B43">
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
       <c r="D43" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="E43" t="s">
-        <v>182</v>
+        <v>198</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="G43" t="s">
         <v>14</v>
       </c>
       <c r="H43" t="s">
-        <v>203</v>
+        <v>218</v>
       </c>
       <c r="I43" t="s">
         <v>16</v>
       </c>
       <c r="J43" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B44">
         <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="D44" t="s">
-        <v>206</v>
+        <v>221</v>
       </c>
       <c r="E44" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>208</v>
+        <v>223</v>
       </c>
       <c r="G44" t="s">
         <v>14</v>
       </c>
       <c r="H44" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
       <c r="I44" t="s">
         <v>16</v>
       </c>
       <c r="J44" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B45">
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>211</v>
+        <v>226</v>
       </c>
       <c r="D45" t="s">
-        <v>212</v>
+        <v>227</v>
       </c>
       <c r="E45" t="s">
         <v>207</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
       <c r="G45" t="s">
         <v>14</v>
       </c>
       <c r="H45" t="s">
-        <v>88</v>
+        <v>228</v>
       </c>
       <c r="I45" t="s">
         <v>16</v>
       </c>
       <c r="J45" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B46">
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>215</v>
+        <v>230</v>
       </c>
       <c r="D46" t="s">
-        <v>216</v>
+        <v>231</v>
       </c>
       <c r="E46" t="s">
         <v>198</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
       <c r="G46" t="s">
         <v>14</v>
       </c>
       <c r="H46" t="s">
-        <v>218</v>
+        <v>232</v>
       </c>
       <c r="I46" t="s">
-        <v>16</v>
+        <v>198</v>
       </c>
       <c r="J46" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B47">
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>220</v>
+        <v>234</v>
       </c>
       <c r="D47" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="E47" t="s">
-        <v>222</v>
+        <v>236</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="G47" t="s">
         <v>14</v>
       </c>
       <c r="H47" t="s">
-        <v>224</v>
-      </c>
-      <c r="I47" t="s">
-        <v>16</v>
-      </c>
-      <c r="J47" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>44</v>
-      </c>
-      <c r="B48">
-        <v>1</v>
-      </c>
-      <c r="C48" t="s">
-        <v>226</v>
-      </c>
-      <c r="D48" t="s">
-        <v>227</v>
-      </c>
-      <c r="E48" t="s">
-        <v>207</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="G48" t="s">
-        <v>14</v>
-      </c>
-      <c r="H48" t="s">
-        <v>228</v>
-      </c>
-      <c r="I48" t="s">
-        <v>16</v>
-      </c>
-      <c r="J48" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>45</v>
-      </c>
-      <c r="B49">
-        <v>1</v>
-      </c>
-      <c r="C49" t="s">
-        <v>230</v>
-      </c>
-      <c r="D49" t="s">
-        <v>231</v>
-      </c>
-      <c r="E49" t="s">
-        <v>198</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="G49" t="s">
-        <v>14</v>
-      </c>
-      <c r="H49" t="s">
-        <v>232</v>
-      </c>
-      <c r="I49" t="s">
-        <v>198</v>
-      </c>
-      <c r="J49" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>46</v>
-      </c>
-      <c r="B50">
-        <v>1</v>
-      </c>
-      <c r="C50" t="s">
-        <v>234</v>
-      </c>
-      <c r="D50" t="s">
-        <v>235</v>
-      </c>
-      <c r="E50" t="s">
-        <v>236</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="G50" t="s">
-        <v>14</v>
-      </c>
-      <c r="H50" t="s">
         <v>237</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="58" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="54" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>

<commit_message>
moving nicoboard to r9
</commit_message>
<xml_diff>
--- a/docs/pcbs/tulip4_board_v4r9/tulipcc-bom.xlsx
+++ b/docs/pcbs/tulip4_board_v4r9/tulipcc-bom.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bwhitman/outside/tulipcc/docs/pcbs/tulip4_board_v4r9/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3E664A-EDF1-4845-A608-31BA59DDE2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="5780" yWindow="1940" windowWidth="32660" windowHeight="21680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="18285" windowHeight="10320"/>
   </bookViews>
   <sheets>
     <sheet name="tulipcc" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -28,16 +22,16 @@
     <t>Qty</t>
   </si>
   <si>
-    <t>Reference(s)</t>
-  </si>
-  <si>
-    <t>Value</t>
+    <t>Designator</t>
+  </si>
+  <si>
+    <t>Comment</t>
   </si>
   <si>
     <t>Manufacturer</t>
   </si>
   <si>
-    <t>Part #</t>
+    <t>Footprint</t>
   </si>
   <si>
     <t>Supplier 1</t>
@@ -130,6 +124,9 @@
     <t>WE</t>
   </si>
   <si>
+    <t>865060345007</t>
+  </si>
+  <si>
     <t>710-865060345007</t>
   </si>
   <si>
@@ -142,6 +139,9 @@
     <t>10uF</t>
   </si>
   <si>
+    <t>865060340001</t>
+  </si>
+  <si>
     <t>710-865060340001</t>
   </si>
   <si>
@@ -286,384 +286,405 @@
     <t>SJ2-35863B1-SMT-TR</t>
   </si>
   <si>
+    <t>490-SJ2-35863B1SMTTR</t>
+  </si>
+  <si>
+    <t>CP-SJ2-35863B1-SMT-CT-ND</t>
+  </si>
+  <si>
+    <t>J8</t>
+  </si>
+  <si>
+    <t>1734827-2</t>
+  </si>
+  <si>
+    <t>571-1734827-2</t>
+  </si>
+  <si>
+    <t>455-S2B-PH-SM4-TBCT-ND</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>1uH</t>
+  </si>
+  <si>
+    <t>Vishay Dale</t>
+  </si>
+  <si>
+    <t>IFSC1515AHER1R0M01</t>
+  </si>
+  <si>
+    <t>70-IFSC1515AHER1R0M0</t>
+  </si>
+  <si>
+    <t>541-1403-1-ND</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>DMP3099L</t>
+  </si>
+  <si>
+    <t>DMP3099L-13</t>
+  </si>
+  <si>
+    <t>621-DMP3099L-13</t>
+  </si>
+  <si>
+    <t>DMP3099L-13DICT-ND</t>
+  </si>
+  <si>
+    <t>R1, R2, R11, R14, R27, R28, R30, R31, R32</t>
+  </si>
+  <si>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>Bourns</t>
+  </si>
+  <si>
+    <t>CR0805-FX-1002ELF</t>
+  </si>
+  <si>
+    <t>652-CR0805FX-1002ELF</t>
+  </si>
+  <si>
+    <t>CR0805-FX-1002ELFCT-ND</t>
+  </si>
+  <si>
+    <t>R3, R4</t>
+  </si>
+  <si>
+    <t>2.4K</t>
+  </si>
+  <si>
+    <t>CR0805-FX-2401ELF</t>
+  </si>
+  <si>
+    <t>652-CR0805FX-2401ELF</t>
+  </si>
+  <si>
+    <t>CR0805-FX-2401ELFCT-ND</t>
+  </si>
+  <si>
+    <t>R5, R6</t>
+  </si>
+  <si>
+    <t>100K</t>
+  </si>
+  <si>
+    <t>CR0805-FX-1003ELF</t>
+  </si>
+  <si>
+    <t>652-CR0805FX-1003ELF</t>
+  </si>
+  <si>
+    <t>CR0805-FX-1003ELFCT-ND</t>
+  </si>
+  <si>
+    <t>R7, R8</t>
+  </si>
+  <si>
+    <t>27R</t>
+  </si>
+  <si>
+    <t>CR0805-FX-27R0ELF</t>
+  </si>
+  <si>
+    <t>652-CR0805FX-27R0ELF</t>
+  </si>
+  <si>
+    <t>118-CMP0603AFX-27R0ELFCT-ND</t>
+  </si>
+  <si>
+    <t>R9, R10</t>
+  </si>
+  <si>
+    <t>5.1K</t>
+  </si>
+  <si>
+    <t>CR0805-FX-5101ELF</t>
+  </si>
+  <si>
+    <t>652-CR0805FX-5101ELF</t>
+  </si>
+  <si>
+    <t>CR0805-FX-5101ELFCT-ND</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>220R</t>
+  </si>
+  <si>
+    <t>CR0805-FX-2200ELF</t>
+  </si>
+  <si>
+    <t>652-CR0805FX-2200ELF</t>
+  </si>
+  <si>
+    <t>CR0805-FX-2200ELFCT-ND</t>
+  </si>
+  <si>
+    <t>R13, R22, R23</t>
+  </si>
+  <si>
+    <t>470R</t>
+  </si>
+  <si>
+    <t>CR0805-FX-4700ELF</t>
+  </si>
+  <si>
+    <t>652-CR0805FX-4700ELF</t>
+  </si>
+  <si>
+    <t>CR0805-FX-4700ELFCT-ND</t>
+  </si>
+  <si>
+    <t>R15, R16</t>
+  </si>
+  <si>
+    <t>0R</t>
+  </si>
+  <si>
+    <t>CR0805-J/-000ELF</t>
+  </si>
+  <si>
+    <t>652-CR0805-J/-000ELF</t>
+  </si>
+  <si>
+    <t>CR0805-J/-000ELFCT-ND</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>33R</t>
+  </si>
+  <si>
+    <t>CR0805-FX-3002ELF</t>
+  </si>
+  <si>
+    <t>652-CR0805FX-33R0ELF</t>
+  </si>
+  <si>
+    <t>118-CR0805-FX-3002ELFCT-ND</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>10R</t>
+  </si>
+  <si>
+    <t>CR0805-FX-10R0ELF</t>
+  </si>
+  <si>
+    <t>652-CR0805FX-10R0ELF</t>
+  </si>
+  <si>
+    <t>118-CR0805-FX-10R0ELFCT-ND</t>
+  </si>
+  <si>
+    <t>R19, R20</t>
+  </si>
+  <si>
+    <t>56K</t>
+  </si>
+  <si>
+    <t>CR0805-FX-5602ELF</t>
+  </si>
+  <si>
+    <t>652-CR0805FX-5602ELF</t>
+  </si>
+  <si>
+    <t>118-CR0805-FX-5602ELFCT-ND</t>
+  </si>
+  <si>
+    <t>R21, R26</t>
+  </si>
+  <si>
+    <t>33K</t>
+  </si>
+  <si>
+    <t>CR0805-FX-3302ELF</t>
+  </si>
+  <si>
+    <t>652-CR0805FX-3302ELF</t>
+  </si>
+  <si>
+    <t>CR0805-FX-3302ELFCT-ND</t>
+  </si>
+  <si>
+    <t>R24, R25</t>
+  </si>
+  <si>
+    <t>22K</t>
+  </si>
+  <si>
+    <t>CR0805-FX-2202ELF</t>
+  </si>
+  <si>
+    <t>652-CR0805-FX2202ELF</t>
+  </si>
+  <si>
+    <t>CR0805-FX-2202ELFCT-ND</t>
+  </si>
+  <si>
+    <t>R29</t>
+  </si>
+  <si>
+    <t>2K</t>
+  </si>
+  <si>
+    <t>CR0805-FX-2001ELF</t>
+  </si>
+  <si>
+    <t>652-CR0805FX-2001ELF</t>
+  </si>
+  <si>
+    <t>CR0805-FX-2001ELFCT-ND</t>
+  </si>
+  <si>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>JS102011JAQN</t>
+  </si>
+  <si>
+    <t>C&amp;K</t>
+  </si>
+  <si>
+    <t>611-JS102011JAQN</t>
+  </si>
+  <si>
+    <t>CKN10720CT-ND</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>ESP32-S3-WROOM-2-N32R8V</t>
+  </si>
+  <si>
+    <t>Espressif</t>
+  </si>
+  <si>
+    <t>356-ESP3S3WRM2N32R8V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1965-ESP32-S3-WROOM-2-N32R8VCT-ND </t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>MBT3904DW1T1G</t>
+  </si>
+  <si>
+    <t>Onsemi</t>
+  </si>
+  <si>
+    <t>863-MBT3904DW1T1G</t>
+  </si>
+  <si>
+    <t>MBT3904DW1T1GOSCT-ND</t>
+  </si>
+  <si>
+    <t>U3, U7</t>
+  </si>
+  <si>
+    <t>USBLC6-2SC6</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>511-USBLC6-2SC6</t>
+  </si>
+  <si>
+    <t>497-5235-1-ND</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>FT231XS</t>
+  </si>
+  <si>
+    <t>FTDI</t>
+  </si>
+  <si>
+    <t>FT231XS-R</t>
+  </si>
+  <si>
+    <t>895-FT231XS-R</t>
+  </si>
+  <si>
+    <t>768-1129-1-ND</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>MIC2005A-2YM5-TR</t>
+  </si>
+  <si>
+    <t>Microchip</t>
+  </si>
+  <si>
+    <t>998-MIC2005A-2YM5TR</t>
+  </si>
+  <si>
+    <t>576-3464-1-ND</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>H11L1SR2M</t>
+  </si>
+  <si>
+    <t>512-H11L1SR2M</t>
+  </si>
+  <si>
+    <t>H11L1SR2MCT-ND</t>
+  </si>
+  <si>
+    <t>U8</t>
+  </si>
+  <si>
+    <t>PCM5101A-Q1</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>PCM5101AQPWRQ1</t>
+  </si>
+  <si>
+    <t>595-PCM5101AQPWRQ1</t>
+  </si>
+  <si>
+    <t>296-37276-1-ND</t>
+  </si>
+  <si>
+    <t>U9</t>
+  </si>
+  <si>
+    <t>TPA6110A2DGN</t>
+  </si>
+  <si>
+    <t>TPA6110A2DGNR</t>
+  </si>
+  <si>
     <t>595-TPA6110A2DGNR</t>
   </si>
   <si>
-    <t>CP-SJ2-35863B1-SMT-CT-ND</t>
-  </si>
-  <si>
-    <t>J8</t>
-  </si>
-  <si>
-    <t>1734827-2</t>
-  </si>
-  <si>
-    <t>571-1734827-2</t>
-  </si>
-  <si>
-    <t>455-S2B-PH-SM4-TBCT-ND</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>1uH</t>
-  </si>
-  <si>
-    <t>Vishay Dale</t>
-  </si>
-  <si>
-    <t>IFSC1515AHER1R0M01</t>
-  </si>
-  <si>
-    <t>70-IFSC1515AHER1R0M0</t>
-  </si>
-  <si>
-    <t>541-1403-1-ND</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>DMP3099L</t>
-  </si>
-  <si>
-    <t>DMP3099L-13</t>
-  </si>
-  <si>
-    <t>621-DMP3099L-13</t>
-  </si>
-  <si>
-    <t>DMP3099L-13DICT-ND</t>
-  </si>
-  <si>
-    <t>R1, R2, R11, R14, R27, R28, R30, R31, R32</t>
-  </si>
-  <si>
-    <t>10K</t>
-  </si>
-  <si>
-    <t>Bourns</t>
-  </si>
-  <si>
-    <t>CR0805-FX-1002ELF</t>
-  </si>
-  <si>
-    <t>652-CR0805FX-1002ELF</t>
-  </si>
-  <si>
-    <t>CR0805-FX-1002ELFCT-ND</t>
-  </si>
-  <si>
-    <t>R3, R4</t>
-  </si>
-  <si>
-    <t>2.4K</t>
-  </si>
-  <si>
-    <t>CR0805-FX-2401ELF</t>
-  </si>
-  <si>
-    <t>652-CR0805FX-2401ELF</t>
-  </si>
-  <si>
-    <t>CR0805-FX-2401ELFCT-ND</t>
-  </si>
-  <si>
-    <t>R5, R6</t>
-  </si>
-  <si>
-    <t>100K</t>
-  </si>
-  <si>
-    <t>CR0805-FX-1003ELF</t>
-  </si>
-  <si>
-    <t>652-CR0805FX-1003ELF</t>
-  </si>
-  <si>
-    <t>CR0805-FX-1003ELFCT-ND</t>
-  </si>
-  <si>
-    <t>R7, R8</t>
-  </si>
-  <si>
-    <t>27R</t>
-  </si>
-  <si>
-    <t>CR0805-FX-27R0ELF</t>
-  </si>
-  <si>
-    <t>652-CR0805FX-27R0ELF</t>
-  </si>
-  <si>
-    <t>118-CMP0603AFX-27R0ELFCT-ND</t>
-  </si>
-  <si>
-    <t>R9, R10</t>
-  </si>
-  <si>
-    <t>5.1K</t>
-  </si>
-  <si>
-    <t>CR0805-FX-5101ELF</t>
-  </si>
-  <si>
-    <t>652-CR0805FX-5101ELF</t>
-  </si>
-  <si>
-    <t>CR0805-FX-5101ELFCT-ND</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>220R</t>
-  </si>
-  <si>
-    <t>CR0805-FX-2200ELF</t>
-  </si>
-  <si>
-    <t>652-CR0805FX-2200ELF</t>
-  </si>
-  <si>
-    <t>CR0805-FX-2200ELFCT-ND</t>
-  </si>
-  <si>
-    <t>R13, R22, R23</t>
-  </si>
-  <si>
-    <t>470R</t>
-  </si>
-  <si>
-    <t>R15, R16</t>
-  </si>
-  <si>
-    <t>0R</t>
-  </si>
-  <si>
-    <t>CR0805-J/-000ELF</t>
-  </si>
-  <si>
-    <t>652-CR0805-J/-000ELF</t>
-  </si>
-  <si>
-    <t>CR0805-J/-000ELFCT-ND</t>
-  </si>
-  <si>
-    <t>R17</t>
-  </si>
-  <si>
-    <t>33R</t>
-  </si>
-  <si>
-    <t>CR0805-FX-3002ELF</t>
-  </si>
-  <si>
-    <t>652-CR0805FX-33R0ELF</t>
-  </si>
-  <si>
-    <t>118-CR0805-FX-3002ELFCT-ND</t>
-  </si>
-  <si>
-    <t>R18</t>
-  </si>
-  <si>
-    <t>10R</t>
-  </si>
-  <si>
-    <t>CR0805-FX-10R0ELF</t>
-  </si>
-  <si>
-    <t>652-CR0805FX-10R0ELF</t>
-  </si>
-  <si>
-    <t>118-CR0805-FX-10R0ELFCT-ND</t>
-  </si>
-  <si>
-    <t>R19, R20</t>
-  </si>
-  <si>
-    <t>56K</t>
-  </si>
-  <si>
-    <t>CR0805-FX-5602ELF</t>
-  </si>
-  <si>
-    <t>652-CR0805FX-5602ELF</t>
-  </si>
-  <si>
-    <t>118-CR0805-FX-5602ELFCT-ND</t>
-  </si>
-  <si>
-    <t>R21, R26</t>
-  </si>
-  <si>
-    <t>33K</t>
-  </si>
-  <si>
-    <t>R24, R25</t>
-  </si>
-  <si>
-    <t>22K</t>
-  </si>
-  <si>
-    <t>CR0805-FX-2202ELF</t>
-  </si>
-  <si>
-    <t>652-CR0805-FX2202ELF</t>
-  </si>
-  <si>
-    <t>CR0805-FX-2202ELFCT-ND</t>
-  </si>
-  <si>
-    <t>R29</t>
-  </si>
-  <si>
-    <t>2K</t>
-  </si>
-  <si>
-    <t>CR0805-FX-2001ELF</t>
-  </si>
-  <si>
-    <t>652-CR0805FX-2001ELF</t>
-  </si>
-  <si>
-    <t>CR0805-FX-2001ELFCT-ND</t>
-  </si>
-  <si>
-    <t>SW1</t>
-  </si>
-  <si>
-    <t>JS102011JAQN</t>
-  </si>
-  <si>
-    <t>C&amp;K</t>
-  </si>
-  <si>
-    <t>611-JS102011JAQN</t>
-  </si>
-  <si>
-    <t>CKN10720CT-ND</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>ESP32-S3-WROOM-2-N32R8V</t>
-  </si>
-  <si>
-    <t>Espressif</t>
-  </si>
-  <si>
-    <t>356-ESP3S3WRM2N32R8V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1965-ESP32-S3-WROOM-2-N32R8VCT-ND </t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>MBT3904DW1T1G</t>
-  </si>
-  <si>
-    <t>Onsemi</t>
-  </si>
-  <si>
-    <t>863-MBT3904DW1T1G</t>
-  </si>
-  <si>
-    <t>MBT3904DW1T1GOSCT-ND</t>
-  </si>
-  <si>
-    <t>U3, U7</t>
-  </si>
-  <si>
-    <t>USBLC6-2SC6</t>
-  </si>
-  <si>
-    <t>ST</t>
-  </si>
-  <si>
-    <t>511-USBLC6-2SC6</t>
-  </si>
-  <si>
-    <t>497-5235-1-ND</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>FT231XS</t>
-  </si>
-  <si>
-    <t>FTDI</t>
-  </si>
-  <si>
-    <t>FT231XS-R</t>
-  </si>
-  <si>
-    <t>895-FT231XS-R</t>
-  </si>
-  <si>
-    <t>768-1129-1-ND</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>MIC2005A-2YM5-TR</t>
-  </si>
-  <si>
-    <t>Microchip</t>
-  </si>
-  <si>
-    <t>998-MIC2005A-2YM5TR</t>
-  </si>
-  <si>
-    <t>576-3464-1-ND</t>
-  </si>
-  <si>
-    <t>U6</t>
-  </si>
-  <si>
-    <t>H11L1SR2M</t>
-  </si>
-  <si>
-    <t>512-H11L1SR2M</t>
-  </si>
-  <si>
-    <t>H11L1SR2MCT-ND</t>
-  </si>
-  <si>
-    <t>U8</t>
-  </si>
-  <si>
-    <t>PCM5101A-Q1</t>
-  </si>
-  <si>
-    <t>TI</t>
-  </si>
-  <si>
-    <t>PCM5101AQPWRQ1</t>
-  </si>
-  <si>
-    <t>595-PCM5101AQPWRQ1</t>
-  </si>
-  <si>
-    <t>296-37276-1-ND</t>
-  </si>
-  <si>
-    <t>U9</t>
-  </si>
-  <si>
-    <t>TPA6110A2DGN</t>
-  </si>
-  <si>
-    <t>TPA6110A2DGNR</t>
-  </si>
-  <si>
     <t>296-31976-1-ND</t>
   </si>
   <si>
@@ -734,179 +755,174 @@
   </si>
   <si>
     <t>688-RK10J12R0A0B</t>
-  </si>
-  <si>
-    <t>865060345007</t>
-  </si>
-  <si>
-    <t>865060340001</t>
-  </si>
-  <si>
-    <t>CR0805-FX-3302ELF</t>
-  </si>
-  <si>
-    <t>652-CR0805FX-3302ELF</t>
-  </si>
-  <si>
-    <t>CR0805-FX-3302ELFCT-ND</t>
-  </si>
-  <si>
-    <t>CR0805-FX-4700ELF</t>
-  </si>
-  <si>
-    <t>652-CR0805FX-4700ELF</t>
-  </si>
-  <si>
-    <t>CR0805-FX-4700ELFCT-ND</t>
-  </si>
-  <si>
-    <t>490-SJ2-35863B1SMTTR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
+      <name val="等线 Light"/>
+      <charset val="134"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -918,175 +934,188 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1096,6 +1125,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1121,7 +1165,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color theme="4" tint="0.399975585192419"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1156,15 +1200,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1180,17 +1215,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1206,102 +1235,130 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+  <cellStyles count="49">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="49" formatCode="@"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1309,27 +1366,24 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J47" totalsRowShown="0">
-  <autoFilter ref="A1:J47" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J47" totalsRowShown="0">
+  <autoFilter ref="A1:J47"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Item"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Qty"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Reference(s)"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Value"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Manufacturer"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Part #" dataDxfId="0"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Supplier 1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Supplier 1 #"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Supplier 2"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Supplier 2 #"/>
+    <tableColumn id="1" name="Item"/>
+    <tableColumn id="2" name="Qty"/>
+    <tableColumn id="3" name="Designator"/>
+    <tableColumn id="4" name="Comment"/>
+    <tableColumn id="5" name="Manufacturer"/>
+    <tableColumn id="6" name="Footprint" dataDxfId="0"/>
+    <tableColumn id="8" name="Supplier 1"/>
+    <tableColumn id="9" name="Supplier 1 #"/>
+    <tableColumn id="10" name="Supplier 2"/>
+    <tableColumn id="11" name="Supplier 2 #"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1378,7 +1432,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1411,26 +1465,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1463,23 +1500,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1621,41 +1641,35 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83333333333333" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.66666666666667" customWidth="1"/>
+    <col min="2" max="2" width="6.33333333333333" customWidth="1"/>
+    <col min="3" max="3" width="42.6666666666667" customWidth="1"/>
+    <col min="4" max="4" width="27" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="27" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27" style="1" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" customWidth="1"/>
-    <col min="10" max="10" width="36.83203125" customWidth="1"/>
+    <col min="8" max="8" width="23.8333333333333" customWidth="1"/>
+    <col min="9" max="9" width="11.6666666666667" customWidth="1"/>
+    <col min="10" max="10" width="36.8333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1687,7 +1701,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1719,7 +1733,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1751,7 +1765,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1783,7 +1797,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1815,7 +1829,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1832,22 +1846,22 @@
         <v>35</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>238</v>
+        <v>36</v>
       </c>
       <c r="G6" t="s">
         <v>14</v>
       </c>
       <c r="H6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I6" t="s">
         <v>16</v>
       </c>
       <c r="J6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1855,31 +1869,31 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E7" t="s">
         <v>35</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>239</v>
+        <v>41</v>
       </c>
       <c r="G7" t="s">
         <v>14</v>
       </c>
       <c r="H7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I7" t="s">
         <v>16</v>
       </c>
       <c r="J7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1887,31 +1901,31 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G8" t="s">
         <v>14</v>
       </c>
       <c r="H8" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I8" t="s">
         <v>16</v>
       </c>
       <c r="J8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1919,31 +1933,31 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G9" t="s">
         <v>14</v>
       </c>
       <c r="H9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I9" t="s">
         <v>16</v>
       </c>
       <c r="J9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1951,31 +1965,31 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G10" t="s">
         <v>14</v>
       </c>
       <c r="H10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I10" t="s">
         <v>16</v>
       </c>
       <c r="J10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1983,31 +1997,31 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E11" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G11" t="s">
         <v>14</v>
       </c>
       <c r="H11" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I11" t="s">
         <v>16</v>
       </c>
       <c r="J11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2015,31 +2029,31 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E12" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G12" t="s">
         <v>14</v>
       </c>
       <c r="H12" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I12" t="s">
         <v>16</v>
       </c>
       <c r="J12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2047,31 +2061,31 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E13" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G13" t="s">
         <v>14</v>
       </c>
       <c r="H13" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I13" t="s">
         <v>16</v>
       </c>
       <c r="J13" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2079,31 +2093,31 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D14" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E14" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G14" t="s">
         <v>14</v>
       </c>
       <c r="H14" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="I14" t="s">
         <v>16</v>
       </c>
       <c r="J14" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2111,31 +2125,31 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D15" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E15" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G15" t="s">
         <v>14</v>
       </c>
       <c r="H15" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I15" t="s">
         <v>16</v>
       </c>
       <c r="J15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" ht="16.5" spans="1:10">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2143,31 +2157,31 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D16" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E16" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G16" t="s">
         <v>14</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>246</v>
+        <v>90</v>
       </c>
       <c r="I16" t="s">
         <v>16</v>
       </c>
       <c r="J16" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2175,31 +2189,31 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D17" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E17" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G17" t="s">
         <v>14</v>
       </c>
       <c r="H17" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I17" t="s">
         <v>16</v>
       </c>
       <c r="J17" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2207,31 +2221,31 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E18" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="G18" t="s">
         <v>14</v>
       </c>
       <c r="H18" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="I18" t="s">
         <v>16</v>
       </c>
       <c r="J18" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2239,31 +2253,31 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D19" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E19" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G19" t="s">
         <v>14</v>
       </c>
       <c r="H19" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I19" t="s">
         <v>16</v>
       </c>
       <c r="J19" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2271,31 +2285,31 @@
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D20" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E20" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G20" t="s">
         <v>14</v>
       </c>
       <c r="H20" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="I20" t="s">
         <v>16</v>
       </c>
       <c r="J20" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2303,31 +2317,31 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D21" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E21" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G21" t="s">
         <v>14</v>
       </c>
       <c r="H21" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I21" t="s">
         <v>16</v>
       </c>
       <c r="J21" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2335,31 +2349,31 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D22" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E22" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G22" t="s">
         <v>14</v>
       </c>
       <c r="H22" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="I22" t="s">
         <v>16</v>
       </c>
       <c r="J22" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2367,31 +2381,31 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D23" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E23" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G23" t="s">
         <v>14</v>
       </c>
       <c r="H23" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="I23" t="s">
         <v>16</v>
       </c>
       <c r="J23" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2399,31 +2413,31 @@
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D24" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E24" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="G24" t="s">
         <v>14</v>
       </c>
       <c r="H24" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I24" t="s">
         <v>16</v>
       </c>
       <c r="J24" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2431,31 +2445,31 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D25" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E25" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G25" t="s">
         <v>14</v>
       </c>
       <c r="H25" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="I25" t="s">
         <v>16</v>
       </c>
       <c r="J25" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2463,31 +2477,31 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D26" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E26" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>243</v>
+        <v>140</v>
       </c>
       <c r="G26" t="s">
         <v>14</v>
       </c>
       <c r="H26" t="s">
-        <v>244</v>
+        <v>141</v>
       </c>
       <c r="I26" t="s">
         <v>16</v>
       </c>
       <c r="J26" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2495,31 +2509,31 @@
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="D27" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="E27" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="G27" t="s">
         <v>14</v>
       </c>
       <c r="H27" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="I27" t="s">
         <v>16</v>
       </c>
       <c r="J27" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2527,31 +2541,31 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D28" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="E28" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="G28" t="s">
         <v>14</v>
       </c>
       <c r="H28" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="I28" t="s">
         <v>16</v>
       </c>
       <c r="J28" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2559,31 +2573,31 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="D29" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="E29" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="G29" t="s">
         <v>14</v>
       </c>
       <c r="H29" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="I29" t="s">
         <v>16</v>
       </c>
       <c r="J29" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2591,31 +2605,31 @@
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="D30" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="E30" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="G30" t="s">
         <v>14</v>
       </c>
       <c r="H30" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="I30" t="s">
         <v>16</v>
       </c>
       <c r="J30" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2623,31 +2637,31 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D31" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="E31" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>240</v>
+        <v>165</v>
       </c>
       <c r="G31" t="s">
         <v>14</v>
       </c>
       <c r="H31" t="s">
-        <v>241</v>
+        <v>166</v>
       </c>
       <c r="I31" t="s">
         <v>16</v>
       </c>
       <c r="J31" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2655,31 +2669,31 @@
         <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="D32" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="E32" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="G32" t="s">
         <v>14</v>
       </c>
       <c r="H32" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="I32" t="s">
         <v>16</v>
       </c>
       <c r="J32" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2687,31 +2701,31 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="D33" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="E33" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="G33" t="s">
         <v>14</v>
       </c>
       <c r="H33" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="I33" t="s">
         <v>16</v>
       </c>
       <c r="J33" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2719,31 +2733,31 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="D34" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="E34" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="G34" t="s">
         <v>14</v>
       </c>
       <c r="H34" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="I34" t="s">
         <v>16</v>
       </c>
       <c r="J34" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2751,31 +2765,31 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="D35" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="E35" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="G35" t="s">
         <v>14</v>
       </c>
       <c r="H35" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="I35" t="s">
         <v>16</v>
       </c>
       <c r="J35" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2783,31 +2797,31 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="D36" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="E36" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="G36" t="s">
         <v>14</v>
       </c>
       <c r="H36" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="I36" t="s">
         <v>16</v>
       </c>
       <c r="J36" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2815,31 +2829,31 @@
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="D37" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="E37" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="G37" t="s">
         <v>14</v>
       </c>
       <c r="H37" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="I37" t="s">
         <v>16</v>
       </c>
       <c r="J37" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2847,31 +2861,31 @@
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="D38" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="E38" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="G38" t="s">
         <v>14</v>
       </c>
       <c r="H38" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="I38" t="s">
         <v>16</v>
       </c>
       <c r="J38" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2879,31 +2893,31 @@
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="D39" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="E39" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="G39" t="s">
         <v>14</v>
       </c>
       <c r="H39" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="I39" t="s">
         <v>16</v>
       </c>
       <c r="J39" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2911,31 +2925,31 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="D40" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="E40" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="G40" t="s">
         <v>14</v>
       </c>
       <c r="H40" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="I40" t="s">
         <v>16</v>
       </c>
       <c r="J40" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2943,31 +2957,31 @@
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="D41" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="E41" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="G41" t="s">
         <v>14</v>
       </c>
       <c r="H41" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="I41" t="s">
         <v>16</v>
       </c>
       <c r="J41" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2975,31 +2989,31 @@
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="D42" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="E42" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="G42" t="s">
         <v>14</v>
       </c>
       <c r="H42" t="s">
-        <v>88</v>
+        <v>222</v>
       </c>
       <c r="I42" t="s">
         <v>16</v>
       </c>
       <c r="J42" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3007,31 +3021,31 @@
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="D43" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="E43" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="G43" t="s">
         <v>14</v>
       </c>
       <c r="H43" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="I43" t="s">
         <v>16</v>
       </c>
       <c r="J43" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3039,31 +3053,31 @@
         <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="D44" t="s">
-        <v>221</v>
+        <v>230</v>
       </c>
       <c r="E44" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="G44" t="s">
         <v>14</v>
       </c>
       <c r="H44" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="I44" t="s">
         <v>16</v>
       </c>
       <c r="J44" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3071,31 +3085,31 @@
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="D45" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="E45" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="G45" t="s">
         <v>14</v>
       </c>
       <c r="H45" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="I45" t="s">
         <v>16</v>
       </c>
       <c r="J45" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3103,31 +3117,31 @@
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="D46" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="E46" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="G46" t="s">
         <v>14</v>
       </c>
       <c r="H46" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="I46" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="J46" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3135,29 +3149,30 @@
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="D47" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="E47" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="G47" t="s">
         <v>14</v>
       </c>
       <c r="H47" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="54" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="1" scale="54" orientation="landscape"/>
+  <headerFooter/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>